<commit_message>
implmentacion final mejorando velocidad con copia del funcional
</commit_message>
<xml_diff>
--- a/output/tel_verif/tel_verificacion.xlsx
+++ b/output/tel_verif/tel_verificacion.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,20 +458,56 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>70287670</t>
+          <t>1048018746</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ALVARO DE JESUS MARIN VARGAS</t>
+          <t>JOHAN CAMILO PEREZ SEPULVEDA</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>3178935198</t>
+          <t>3104463513</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1040328596</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>MARIA ISABEL ARANGO TOBON</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>3183779584</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1001471005</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>MARIA LUCEIDA ZAPATA SERNA</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>3234676758</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>